<commit_message>
Part B and C
</commit_message>
<xml_diff>
--- a/Part b (09-19)/NMDS (Metrics and IBI) - B1, 7, 10, REF 12-19/metric_ibi_combined.xlsx
+++ b/Part b (09-19)/NMDS (Metrics and IBI) - B1, 7, 10, REF 12-19/metric_ibi_combined.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub Projects\thesis-codes\Part b (09-19)\NMDS (Metrics and IBI) - B1, 7, 10, REF 12-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE92BF1-0C40-4D05-A57E-DE6021963AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA15CCA3-49FD-475D-8E17-B7C86268C25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metric &amp; IBI" sheetId="5" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
   <si>
     <t>Year</t>
   </si>
@@ -487,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9F43FB-E229-4B7A-802A-753A16EAAB2C}">
-  <dimension ref="A1:FZ21"/>
+  <dimension ref="A1:FZ25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3474,211 +3474,211 @@
         <v>2</v>
       </c>
       <c r="B18">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D18">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G18">
-        <v>2.98</v>
+        <v>3.97</v>
       </c>
       <c r="H18">
-        <v>40.299999999999997</v>
+        <v>42.06</v>
       </c>
       <c r="I18">
-        <v>79.099999999999994</v>
+        <v>71.42</v>
       </c>
       <c r="J18">
-        <v>3.33</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="2"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
-      <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="2"/>
-      <c r="Z18" s="2"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AD18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AF18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AH18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AJ18" s="2"/>
-      <c r="AK18" s="2"/>
-      <c r="AL18" s="2"/>
-      <c r="AM18" s="2"/>
-      <c r="AN18" s="2"/>
-      <c r="AO18" s="2"/>
-      <c r="AP18" s="2"/>
-      <c r="AQ18" s="2"/>
-      <c r="AR18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AT18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AV18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AX18" s="2"/>
-      <c r="AY18" s="2"/>
-      <c r="AZ18" s="2"/>
-      <c r="BA18" s="2"/>
-      <c r="BB18" s="2"/>
-      <c r="BC18" s="2"/>
-      <c r="BD18" s="2"/>
-      <c r="BE18" s="2"/>
-      <c r="BF18" s="2"/>
-      <c r="BG18" s="2"/>
-      <c r="BH18" s="2"/>
-      <c r="BI18" s="2"/>
-      <c r="BJ18" s="2"/>
-      <c r="BK18" s="2"/>
-      <c r="BL18" s="2"/>
-      <c r="BM18" s="2"/>
-      <c r="BN18" s="2"/>
-      <c r="BO18" s="2"/>
-      <c r="BP18" s="2"/>
-      <c r="BQ18" s="2"/>
-      <c r="BR18" s="2"/>
-      <c r="BS18" s="2"/>
-      <c r="BT18" s="2"/>
-      <c r="BU18" s="2"/>
-      <c r="BV18" s="2"/>
-      <c r="BW18" s="2"/>
-      <c r="BX18" s="2"/>
-      <c r="BY18" s="2"/>
-      <c r="BZ18" s="2"/>
-      <c r="CA18" s="2"/>
-      <c r="CB18" s="2"/>
-      <c r="CC18" s="2"/>
-      <c r="CD18" s="2"/>
-      <c r="CE18" s="2"/>
-      <c r="CF18" s="2"/>
-      <c r="CG18" s="2"/>
-      <c r="CH18" s="2"/>
-      <c r="CI18" s="2"/>
-      <c r="CJ18" s="2"/>
-      <c r="CK18" s="2"/>
-      <c r="CL18" s="2"/>
-      <c r="CM18" s="2"/>
-      <c r="CN18" s="2"/>
-      <c r="CO18" s="2"/>
-      <c r="CP18" s="2"/>
-      <c r="CQ18" s="2"/>
-      <c r="CR18" s="2"/>
-      <c r="CS18" s="2"/>
-      <c r="CT18" s="2"/>
-      <c r="CU18" s="2"/>
-      <c r="CV18" s="2"/>
-      <c r="CW18" s="2"/>
-      <c r="CX18" s="2"/>
-      <c r="CY18" s="2"/>
-      <c r="CZ18" s="2"/>
-      <c r="DA18" s="2"/>
-      <c r="DB18" s="2"/>
-      <c r="DC18" s="2"/>
-      <c r="DD18" s="2"/>
-      <c r="DE18" s="2"/>
-      <c r="DF18" s="2"/>
-      <c r="DG18" s="2"/>
-      <c r="DH18" s="2"/>
-      <c r="DI18" s="2"/>
-      <c r="DJ18" s="2"/>
-      <c r="DK18" s="2"/>
-      <c r="DL18" s="2"/>
-      <c r="DM18" s="2"/>
-      <c r="DN18" s="2"/>
-      <c r="DO18" s="2"/>
-      <c r="DP18" s="2"/>
-      <c r="DQ18" s="2"/>
-      <c r="DR18" s="2"/>
-      <c r="DS18" s="2"/>
-      <c r="DT18" s="2"/>
-      <c r="DU18" s="2"/>
-      <c r="DV18" s="2"/>
-      <c r="DW18" s="2"/>
-      <c r="DX18" s="2"/>
-      <c r="DY18" s="2"/>
-      <c r="DZ18" s="2"/>
-      <c r="EA18" s="2"/>
-      <c r="EB18" s="2"/>
-      <c r="EC18" s="2"/>
-      <c r="ED18" s="2"/>
-      <c r="EE18" s="2"/>
-      <c r="EF18" s="2"/>
-      <c r="EG18" s="2"/>
-      <c r="EH18" s="2"/>
-      <c r="EI18" s="2"/>
-      <c r="EJ18" s="2"/>
-      <c r="EK18" s="2"/>
-      <c r="EL18" s="2"/>
-      <c r="EM18" s="2"/>
-      <c r="EN18" s="2"/>
-      <c r="EO18" s="2"/>
-      <c r="EP18" s="2"/>
-      <c r="EQ18" s="2"/>
-      <c r="ER18" s="2"/>
-      <c r="ES18" s="2"/>
-      <c r="ET18" s="2"/>
-      <c r="EU18" s="2"/>
-      <c r="EV18" s="2"/>
-      <c r="EW18" s="2"/>
-      <c r="EX18" s="2"/>
-      <c r="EY18" s="2"/>
-      <c r="EZ18" s="2"/>
-      <c r="FA18" s="2"/>
-      <c r="FB18" s="2"/>
-      <c r="FC18" s="2"/>
-      <c r="FD18" s="2"/>
-      <c r="FE18" s="2"/>
-      <c r="FF18" s="2"/>
-      <c r="FG18" s="2"/>
-      <c r="FH18" s="2"/>
-      <c r="FI18" s="2"/>
-      <c r="FJ18" s="2"/>
-      <c r="FK18" s="2"/>
-      <c r="FL18" s="2"/>
-      <c r="FM18" s="2"/>
-      <c r="FN18" s="2"/>
-      <c r="FO18" s="2"/>
-      <c r="FP18" s="2"/>
-      <c r="FQ18" s="2"/>
-      <c r="FR18" s="2"/>
-      <c r="FS18" s="2"/>
-      <c r="FT18" s="2"/>
-      <c r="FU18" s="2"/>
-      <c r="FV18" s="2"/>
-      <c r="FW18" s="2"/>
-      <c r="FX18" s="2"/>
-      <c r="FY18" s="2"/>
-      <c r="FZ18" s="2"/>
+        <v>2.33</v>
+      </c>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="4"/>
+      <c r="AP18" s="4"/>
+      <c r="AQ18" s="4"/>
+      <c r="AR18" s="4"/>
+      <c r="AS18" s="4"/>
+      <c r="AT18" s="4"/>
+      <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="4"/>
+      <c r="AX18" s="4"/>
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="4"/>
+      <c r="BB18" s="4"/>
+      <c r="BC18" s="4"/>
+      <c r="BD18" s="4"/>
+      <c r="BE18" s="4"/>
+      <c r="BF18" s="4"/>
+      <c r="BG18" s="4"/>
+      <c r="BH18" s="4"/>
+      <c r="BI18" s="4"/>
+      <c r="BJ18" s="4"/>
+      <c r="BK18" s="4"/>
+      <c r="BL18" s="4"/>
+      <c r="BM18" s="4"/>
+      <c r="BN18" s="4"/>
+      <c r="BO18" s="4"/>
+      <c r="BP18" s="4"/>
+      <c r="BQ18" s="4"/>
+      <c r="BR18" s="4"/>
+      <c r="BS18" s="4"/>
+      <c r="BT18" s="4"/>
+      <c r="BU18" s="4"/>
+      <c r="BV18" s="4"/>
+      <c r="BW18" s="4"/>
+      <c r="BX18" s="4"/>
+      <c r="BY18" s="4"/>
+      <c r="BZ18" s="4"/>
+      <c r="CA18" s="4"/>
+      <c r="CB18" s="4"/>
+      <c r="CC18" s="4"/>
+      <c r="CD18" s="4"/>
+      <c r="CE18" s="4"/>
+      <c r="CF18" s="4"/>
+      <c r="CG18" s="4"/>
+      <c r="CH18" s="4"/>
+      <c r="CI18" s="4"/>
+      <c r="CJ18" s="4"/>
+      <c r="CK18" s="4"/>
+      <c r="CL18" s="4"/>
+      <c r="CM18" s="4"/>
+      <c r="CN18" s="4"/>
+      <c r="CO18" s="4"/>
+      <c r="CP18" s="4"/>
+      <c r="CQ18" s="4"/>
+      <c r="CR18" s="4"/>
+      <c r="CS18" s="4"/>
+      <c r="CT18" s="4"/>
+      <c r="CU18" s="4"/>
+      <c r="CV18" s="4"/>
+      <c r="CW18" s="4"/>
+      <c r="CX18" s="4"/>
+      <c r="CY18" s="4"/>
+      <c r="CZ18" s="4"/>
+      <c r="DA18" s="4"/>
+      <c r="DB18" s="4"/>
+      <c r="DC18" s="4"/>
+      <c r="DD18" s="4"/>
+      <c r="DE18" s="4"/>
+      <c r="DF18" s="4"/>
+      <c r="DG18" s="4"/>
+      <c r="DH18" s="4"/>
+      <c r="DI18" s="4"/>
+      <c r="DJ18" s="4"/>
+      <c r="DK18" s="4"/>
+      <c r="DL18" s="4"/>
+      <c r="DM18" s="4"/>
+      <c r="DN18" s="4"/>
+      <c r="DO18" s="4"/>
+      <c r="DP18" s="4"/>
+      <c r="DQ18" s="4"/>
+      <c r="DR18" s="4"/>
+      <c r="DS18" s="4"/>
+      <c r="DT18" s="4"/>
+      <c r="DU18" s="4"/>
+      <c r="DV18" s="4"/>
+      <c r="DW18" s="4"/>
+      <c r="DX18" s="4"/>
+      <c r="DY18" s="4"/>
+      <c r="DZ18" s="4"/>
+      <c r="EA18" s="4"/>
+      <c r="EB18" s="4"/>
+      <c r="EC18" s="4"/>
+      <c r="ED18" s="4"/>
+      <c r="EE18" s="4"/>
+      <c r="EF18" s="4"/>
+      <c r="EG18" s="4"/>
+      <c r="EH18" s="4"/>
+      <c r="EI18" s="4"/>
+      <c r="EJ18" s="4"/>
+      <c r="EK18" s="4"/>
+      <c r="EL18" s="4"/>
+      <c r="EM18" s="4"/>
+      <c r="EN18" s="4"/>
+      <c r="EO18" s="4"/>
+      <c r="EP18" s="4"/>
+      <c r="EQ18" s="4"/>
+      <c r="ER18" s="4"/>
+      <c r="ES18" s="4"/>
+      <c r="ET18" s="4"/>
+      <c r="EU18" s="4"/>
+      <c r="EV18" s="4"/>
+      <c r="EW18" s="4"/>
+      <c r="EX18" s="4"/>
+      <c r="EY18" s="4"/>
+      <c r="EZ18" s="4"/>
+      <c r="FA18" s="4"/>
+      <c r="FB18" s="4"/>
+      <c r="FC18" s="4"/>
+      <c r="FD18" s="4"/>
+      <c r="FE18" s="4"/>
+      <c r="FF18" s="4"/>
+      <c r="FG18" s="4"/>
+      <c r="FH18" s="4"/>
+      <c r="FI18" s="4"/>
+      <c r="FJ18" s="4"/>
+      <c r="FK18" s="4"/>
+      <c r="FL18" s="4"/>
+      <c r="FM18" s="4"/>
+      <c r="FN18" s="4"/>
+      <c r="FO18" s="4"/>
+      <c r="FP18" s="4"/>
+      <c r="FQ18" s="4"/>
+      <c r="FR18" s="4"/>
+      <c r="FS18" s="4"/>
+      <c r="FT18" s="4"/>
+      <c r="FU18" s="4"/>
+      <c r="FV18" s="4"/>
+      <c r="FW18" s="4"/>
+      <c r="FX18" s="4"/>
+      <c r="FY18" s="4"/>
+      <c r="FZ18" s="4"/>
     </row>
     <row r="19" spans="1:182" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>3</v>
@@ -3687,603 +3687,1419 @@
         <v>22</v>
       </c>
       <c r="E19">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>10.83</v>
       </c>
       <c r="H19">
-        <v>75.319999999999993</v>
+        <v>30.83</v>
       </c>
       <c r="I19">
-        <v>60.13</v>
+        <v>72.5</v>
       </c>
       <c r="J19">
-        <v>1.67</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-      <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="2"/>
-      <c r="Z19" s="2"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AD19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AF19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AH19" s="2"/>
-      <c r="AI19" s="2"/>
-      <c r="AJ19" s="2"/>
-      <c r="AK19" s="2"/>
-      <c r="AL19" s="2"/>
-      <c r="AM19" s="2"/>
-      <c r="AN19" s="2"/>
-      <c r="AO19" s="2"/>
-      <c r="AP19" s="2"/>
-      <c r="AQ19" s="2"/>
-      <c r="AR19" s="2"/>
-      <c r="AS19" s="2"/>
-      <c r="AT19" s="2"/>
-      <c r="AU19" s="2"/>
-      <c r="AV19" s="2"/>
-      <c r="AW19" s="2"/>
-      <c r="AX19" s="2"/>
-      <c r="AY19" s="2"/>
-      <c r="AZ19" s="2"/>
-      <c r="BA19" s="2"/>
-      <c r="BB19" s="2"/>
-      <c r="BC19" s="2"/>
-      <c r="BD19" s="2"/>
-      <c r="BE19" s="2"/>
-      <c r="BF19" s="2"/>
-      <c r="BG19" s="2"/>
-      <c r="BH19" s="2"/>
-      <c r="BI19" s="2"/>
-      <c r="BJ19" s="2"/>
-      <c r="BK19" s="2"/>
-      <c r="BL19" s="2"/>
-      <c r="BM19" s="2"/>
-      <c r="BN19" s="2"/>
-      <c r="BO19" s="2"/>
-      <c r="BP19" s="2"/>
-      <c r="BQ19" s="2"/>
-      <c r="BR19" s="2"/>
-      <c r="BS19" s="2"/>
-      <c r="BT19" s="2"/>
-      <c r="BU19" s="2"/>
-      <c r="BV19" s="2"/>
-      <c r="BW19" s="2"/>
-      <c r="BX19" s="2"/>
-      <c r="BY19" s="2"/>
-      <c r="BZ19" s="2"/>
-      <c r="CA19" s="2"/>
-      <c r="CB19" s="2"/>
-      <c r="CC19" s="2"/>
-      <c r="CD19" s="2"/>
-      <c r="CE19" s="2"/>
-      <c r="CF19" s="2"/>
-      <c r="CG19" s="2"/>
-      <c r="CH19" s="2"/>
-      <c r="CI19" s="2"/>
-      <c r="CJ19" s="2"/>
-      <c r="CK19" s="2"/>
-      <c r="CL19" s="2"/>
-      <c r="CM19" s="2"/>
-      <c r="CN19" s="2"/>
-      <c r="CO19" s="2"/>
-      <c r="CP19" s="2"/>
-      <c r="CQ19" s="2"/>
-      <c r="CR19" s="2"/>
-      <c r="CS19" s="2"/>
-      <c r="CT19" s="2"/>
-      <c r="CU19" s="2"/>
-      <c r="CV19" s="2"/>
-      <c r="CW19" s="2"/>
-      <c r="CX19" s="2"/>
-      <c r="CY19" s="2"/>
-      <c r="CZ19" s="2"/>
-      <c r="DA19" s="2"/>
-      <c r="DB19" s="2"/>
-      <c r="DC19" s="2"/>
-      <c r="DD19" s="2"/>
-      <c r="DE19" s="2"/>
-      <c r="DF19" s="2"/>
-      <c r="DG19" s="2"/>
-      <c r="DH19" s="2"/>
-      <c r="DI19" s="2"/>
-      <c r="DJ19" s="2"/>
-      <c r="DK19" s="2"/>
-      <c r="DL19" s="2"/>
-      <c r="DM19" s="2"/>
-      <c r="DN19" s="2"/>
-      <c r="DO19" s="2"/>
-      <c r="DP19" s="2"/>
-      <c r="DQ19" s="2"/>
-      <c r="DR19" s="2"/>
-      <c r="DS19" s="2"/>
-      <c r="DT19" s="2"/>
-      <c r="DU19" s="2"/>
-      <c r="DV19" s="2"/>
-      <c r="DW19" s="2"/>
-      <c r="DX19" s="2"/>
-      <c r="DY19" s="2"/>
-      <c r="DZ19" s="2"/>
-      <c r="EA19" s="2"/>
-      <c r="EB19" s="2"/>
-      <c r="EC19" s="2"/>
-      <c r="ED19" s="2"/>
-      <c r="EE19" s="2"/>
-      <c r="EF19" s="2"/>
-      <c r="EG19" s="2"/>
-      <c r="EH19" s="2"/>
-      <c r="EI19" s="2"/>
-      <c r="EJ19" s="2"/>
-      <c r="EK19" s="2"/>
-      <c r="EL19" s="2"/>
-      <c r="EM19" s="2"/>
-      <c r="EN19" s="2"/>
-      <c r="EO19" s="2"/>
-      <c r="EP19" s="2"/>
-      <c r="EQ19" s="2"/>
-      <c r="ER19" s="2"/>
-      <c r="ES19" s="2"/>
-      <c r="ET19" s="2"/>
-      <c r="EU19" s="2"/>
-      <c r="EV19" s="2"/>
-      <c r="EW19" s="2"/>
-      <c r="EX19" s="2"/>
-      <c r="EY19" s="2"/>
-      <c r="EZ19" s="2"/>
-      <c r="FA19" s="2"/>
-      <c r="FB19" s="2"/>
-      <c r="FC19" s="2"/>
-      <c r="FD19" s="2"/>
-      <c r="FE19" s="2"/>
-      <c r="FF19" s="2"/>
-      <c r="FG19" s="2"/>
-      <c r="FH19" s="2"/>
-      <c r="FI19" s="2"/>
-      <c r="FJ19" s="2"/>
-      <c r="FK19" s="2"/>
-      <c r="FL19" s="2"/>
-      <c r="FM19" s="2"/>
-      <c r="FN19" s="2"/>
-      <c r="FO19" s="2"/>
-      <c r="FP19" s="2"/>
-      <c r="FQ19" s="2"/>
-      <c r="FR19" s="2"/>
-      <c r="FS19" s="2"/>
-      <c r="FT19" s="2"/>
-      <c r="FU19" s="2"/>
-      <c r="FV19" s="2"/>
-      <c r="FW19" s="2"/>
-      <c r="FX19" s="2"/>
-      <c r="FY19" s="2"/>
-      <c r="FZ19" s="2"/>
+        <v>2.67</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+      <c r="AA19" s="4"/>
+      <c r="AB19" s="4"/>
+      <c r="AC19" s="4"/>
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+      <c r="AG19" s="4"/>
+      <c r="AH19" s="4"/>
+      <c r="AI19" s="4"/>
+      <c r="AJ19" s="4"/>
+      <c r="AK19" s="4"/>
+      <c r="AL19" s="4"/>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="4"/>
+      <c r="AP19" s="4"/>
+      <c r="AQ19" s="4"/>
+      <c r="AR19" s="4"/>
+      <c r="AS19" s="4"/>
+      <c r="AT19" s="4"/>
+      <c r="AU19" s="4"/>
+      <c r="AV19" s="4"/>
+      <c r="AW19" s="4"/>
+      <c r="AX19" s="4"/>
+      <c r="AY19" s="4"/>
+      <c r="AZ19" s="4"/>
+      <c r="BA19" s="4"/>
+      <c r="BB19" s="4"/>
+      <c r="BC19" s="4"/>
+      <c r="BD19" s="4"/>
+      <c r="BE19" s="4"/>
+      <c r="BF19" s="4"/>
+      <c r="BG19" s="4"/>
+      <c r="BH19" s="4"/>
+      <c r="BI19" s="4"/>
+      <c r="BJ19" s="4"/>
+      <c r="BK19" s="4"/>
+      <c r="BL19" s="4"/>
+      <c r="BM19" s="4"/>
+      <c r="BN19" s="4"/>
+      <c r="BO19" s="4"/>
+      <c r="BP19" s="4"/>
+      <c r="BQ19" s="4"/>
+      <c r="BR19" s="4"/>
+      <c r="BS19" s="4"/>
+      <c r="BT19" s="4"/>
+      <c r="BU19" s="4"/>
+      <c r="BV19" s="4"/>
+      <c r="BW19" s="4"/>
+      <c r="BX19" s="4"/>
+      <c r="BY19" s="4"/>
+      <c r="BZ19" s="4"/>
+      <c r="CA19" s="4"/>
+      <c r="CB19" s="4"/>
+      <c r="CC19" s="4"/>
+      <c r="CD19" s="4"/>
+      <c r="CE19" s="4"/>
+      <c r="CF19" s="4"/>
+      <c r="CG19" s="4"/>
+      <c r="CH19" s="4"/>
+      <c r="CI19" s="4"/>
+      <c r="CJ19" s="4"/>
+      <c r="CK19" s="4"/>
+      <c r="CL19" s="4"/>
+      <c r="CM19" s="4"/>
+      <c r="CN19" s="4"/>
+      <c r="CO19" s="4"/>
+      <c r="CP19" s="4"/>
+      <c r="CQ19" s="4"/>
+      <c r="CR19" s="4"/>
+      <c r="CS19" s="4"/>
+      <c r="CT19" s="4"/>
+      <c r="CU19" s="4"/>
+      <c r="CV19" s="4"/>
+      <c r="CW19" s="4"/>
+      <c r="CX19" s="4"/>
+      <c r="CY19" s="4"/>
+      <c r="CZ19" s="4"/>
+      <c r="DA19" s="4"/>
+      <c r="DB19" s="4"/>
+      <c r="DC19" s="4"/>
+      <c r="DD19" s="4"/>
+      <c r="DE19" s="4"/>
+      <c r="DF19" s="4"/>
+      <c r="DG19" s="4"/>
+      <c r="DH19" s="4"/>
+      <c r="DI19" s="4"/>
+      <c r="DJ19" s="4"/>
+      <c r="DK19" s="4"/>
+      <c r="DL19" s="4"/>
+      <c r="DM19" s="4"/>
+      <c r="DN19" s="4"/>
+      <c r="DO19" s="4"/>
+      <c r="DP19" s="4"/>
+      <c r="DQ19" s="4"/>
+      <c r="DR19" s="4"/>
+      <c r="DS19" s="4"/>
+      <c r="DT19" s="4"/>
+      <c r="DU19" s="4"/>
+      <c r="DV19" s="4"/>
+      <c r="DW19" s="4"/>
+      <c r="DX19" s="4"/>
+      <c r="DY19" s="4"/>
+      <c r="DZ19" s="4"/>
+      <c r="EA19" s="4"/>
+      <c r="EB19" s="4"/>
+      <c r="EC19" s="4"/>
+      <c r="ED19" s="4"/>
+      <c r="EE19" s="4"/>
+      <c r="EF19" s="4"/>
+      <c r="EG19" s="4"/>
+      <c r="EH19" s="4"/>
+      <c r="EI19" s="4"/>
+      <c r="EJ19" s="4"/>
+      <c r="EK19" s="4"/>
+      <c r="EL19" s="4"/>
+      <c r="EM19" s="4"/>
+      <c r="EN19" s="4"/>
+      <c r="EO19" s="4"/>
+      <c r="EP19" s="4"/>
+      <c r="EQ19" s="4"/>
+      <c r="ER19" s="4"/>
+      <c r="ES19" s="4"/>
+      <c r="ET19" s="4"/>
+      <c r="EU19" s="4"/>
+      <c r="EV19" s="4"/>
+      <c r="EW19" s="4"/>
+      <c r="EX19" s="4"/>
+      <c r="EY19" s="4"/>
+      <c r="EZ19" s="4"/>
+      <c r="FA19" s="4"/>
+      <c r="FB19" s="4"/>
+      <c r="FC19" s="4"/>
+      <c r="FD19" s="4"/>
+      <c r="FE19" s="4"/>
+      <c r="FF19" s="4"/>
+      <c r="FG19" s="4"/>
+      <c r="FH19" s="4"/>
+      <c r="FI19" s="4"/>
+      <c r="FJ19" s="4"/>
+      <c r="FK19" s="4"/>
+      <c r="FL19" s="4"/>
+      <c r="FM19" s="4"/>
+      <c r="FN19" s="4"/>
+      <c r="FO19" s="4"/>
+      <c r="FP19" s="4"/>
+      <c r="FQ19" s="4"/>
+      <c r="FR19" s="4"/>
+      <c r="FS19" s="4"/>
+      <c r="FT19" s="4"/>
+      <c r="FU19" s="4"/>
+      <c r="FV19" s="4"/>
+      <c r="FW19" s="4"/>
+      <c r="FX19" s="4"/>
+      <c r="FY19" s="4"/>
+      <c r="FZ19" s="4"/>
     </row>
     <row r="20" spans="1:182" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
         <v>3</v>
       </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
       <c r="G20">
-        <v>1.47</v>
+        <v>21.05</v>
       </c>
       <c r="H20">
-        <v>32.35</v>
+        <v>42.98</v>
       </c>
       <c r="I20">
-        <v>79.41</v>
+        <v>72.8</v>
       </c>
       <c r="J20">
-        <v>2.33</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="2"/>
-      <c r="Z20" s="2"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AD20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AF20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AH20" s="2"/>
-      <c r="AI20" s="2"/>
-      <c r="AJ20" s="2"/>
-      <c r="AK20" s="2"/>
-      <c r="AL20" s="2"/>
-      <c r="AM20" s="2"/>
-      <c r="AN20" s="2"/>
-      <c r="AO20" s="2"/>
-      <c r="AP20" s="2"/>
-      <c r="AQ20" s="2"/>
-      <c r="AR20" s="2"/>
-      <c r="AS20" s="2"/>
-      <c r="AT20" s="2"/>
-      <c r="AU20" s="2"/>
-      <c r="AV20" s="2"/>
-      <c r="AW20" s="2"/>
-      <c r="AX20" s="2"/>
-      <c r="AY20" s="2"/>
-      <c r="AZ20" s="2"/>
-      <c r="BA20" s="2"/>
-      <c r="BB20" s="2"/>
-      <c r="BC20" s="2"/>
-      <c r="BD20" s="2"/>
-      <c r="BE20" s="2"/>
-      <c r="BF20" s="2"/>
-      <c r="BG20" s="2"/>
-      <c r="BH20" s="2"/>
-      <c r="BI20" s="2"/>
-      <c r="BJ20" s="2"/>
-      <c r="BK20" s="2"/>
-      <c r="BL20" s="2"/>
-      <c r="BM20" s="2"/>
-      <c r="BN20" s="2"/>
-      <c r="BO20" s="2"/>
-      <c r="BP20" s="2"/>
-      <c r="BQ20" s="2"/>
-      <c r="BR20" s="2"/>
-      <c r="BS20" s="2"/>
-      <c r="BT20" s="2"/>
-      <c r="BU20" s="2"/>
-      <c r="BV20" s="2"/>
-      <c r="BW20" s="2"/>
-      <c r="BX20" s="2"/>
-      <c r="BY20" s="2"/>
-      <c r="BZ20" s="2"/>
-      <c r="CA20" s="2"/>
-      <c r="CB20" s="2"/>
-      <c r="CC20" s="2"/>
-      <c r="CD20" s="2"/>
-      <c r="CE20" s="2"/>
-      <c r="CF20" s="2"/>
-      <c r="CG20" s="2"/>
-      <c r="CH20" s="2"/>
-      <c r="CI20" s="2"/>
-      <c r="CJ20" s="2"/>
-      <c r="CK20" s="2"/>
-      <c r="CL20" s="2"/>
-      <c r="CM20" s="2"/>
-      <c r="CN20" s="2"/>
-      <c r="CO20" s="2"/>
-      <c r="CP20" s="2"/>
-      <c r="CQ20" s="2"/>
-      <c r="CR20" s="2"/>
-      <c r="CS20" s="2"/>
-      <c r="CT20" s="2"/>
-      <c r="CU20" s="2"/>
-      <c r="CV20" s="2"/>
-      <c r="CW20" s="2"/>
-      <c r="CX20" s="2"/>
-      <c r="CY20" s="2"/>
-      <c r="CZ20" s="2"/>
-      <c r="DA20" s="2"/>
-      <c r="DB20" s="2"/>
-      <c r="DC20" s="2"/>
-      <c r="DD20" s="2"/>
-      <c r="DE20" s="2"/>
-      <c r="DF20" s="2"/>
-      <c r="DG20" s="2"/>
-      <c r="DH20" s="2"/>
-      <c r="DI20" s="2"/>
-      <c r="DJ20" s="2"/>
-      <c r="DK20" s="2"/>
-      <c r="DL20" s="2"/>
-      <c r="DM20" s="2"/>
-      <c r="DN20" s="2"/>
-      <c r="DO20" s="2"/>
-      <c r="DP20" s="2"/>
-      <c r="DQ20" s="2"/>
-      <c r="DR20" s="2"/>
-      <c r="DS20" s="2"/>
-      <c r="DT20" s="2"/>
-      <c r="DU20" s="2"/>
-      <c r="DV20" s="2"/>
-      <c r="DW20" s="2"/>
-      <c r="DX20" s="2"/>
-      <c r="DY20" s="2"/>
-      <c r="DZ20" s="2"/>
-      <c r="EA20" s="2"/>
-      <c r="EB20" s="2"/>
-      <c r="EC20" s="2"/>
-      <c r="ED20" s="2"/>
-      <c r="EE20" s="2"/>
-      <c r="EF20" s="2"/>
-      <c r="EG20" s="2"/>
-      <c r="EH20" s="2"/>
-      <c r="EI20" s="2"/>
-      <c r="EJ20" s="2"/>
-      <c r="EK20" s="2"/>
-      <c r="EL20" s="2"/>
-      <c r="EM20" s="2"/>
-      <c r="EN20" s="2"/>
-      <c r="EO20" s="2"/>
-      <c r="EP20" s="2"/>
-      <c r="EQ20" s="2"/>
-      <c r="ER20" s="2"/>
-      <c r="ES20" s="2"/>
-      <c r="ET20" s="2"/>
-      <c r="EU20" s="2"/>
-      <c r="EV20" s="2"/>
-      <c r="EW20" s="2"/>
-      <c r="EX20" s="2"/>
-      <c r="EY20" s="2"/>
-      <c r="EZ20" s="2"/>
-      <c r="FA20" s="2"/>
-      <c r="FB20" s="2"/>
-      <c r="FC20" s="2"/>
-      <c r="FD20" s="2"/>
-      <c r="FE20" s="2"/>
-      <c r="FF20" s="2"/>
-      <c r="FG20" s="2"/>
-      <c r="FH20" s="2"/>
-      <c r="FI20" s="2"/>
-      <c r="FJ20" s="2"/>
-      <c r="FK20" s="2"/>
-      <c r="FL20" s="2"/>
-      <c r="FM20" s="2"/>
-      <c r="FN20" s="2"/>
-      <c r="FO20" s="2"/>
-      <c r="FP20" s="2"/>
-      <c r="FQ20" s="2"/>
-      <c r="FR20" s="2"/>
-      <c r="FS20" s="2"/>
-      <c r="FT20" s="2"/>
-      <c r="FU20" s="2"/>
-      <c r="FV20" s="2"/>
-      <c r="FW20" s="2"/>
-      <c r="FX20" s="2"/>
-      <c r="FY20" s="2"/>
-      <c r="FZ20" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
+      <c r="X20" s="4"/>
+      <c r="Y20" s="4"/>
+      <c r="Z20" s="4"/>
+      <c r="AA20" s="4"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+      <c r="AG20" s="4"/>
+      <c r="AH20" s="4"/>
+      <c r="AI20" s="4"/>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="4"/>
+      <c r="AL20" s="4"/>
+      <c r="AM20" s="4"/>
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="4"/>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="4"/>
+      <c r="AR20" s="4"/>
+      <c r="AS20" s="4"/>
+      <c r="AT20" s="4"/>
+      <c r="AU20" s="4"/>
+      <c r="AV20" s="4"/>
+      <c r="AW20" s="4"/>
+      <c r="AX20" s="4"/>
+      <c r="AY20" s="4"/>
+      <c r="AZ20" s="4"/>
+      <c r="BA20" s="4"/>
+      <c r="BB20" s="4"/>
+      <c r="BC20" s="4"/>
+      <c r="BD20" s="4"/>
+      <c r="BE20" s="4"/>
+      <c r="BF20" s="4"/>
+      <c r="BG20" s="4"/>
+      <c r="BH20" s="4"/>
+      <c r="BI20" s="4"/>
+      <c r="BJ20" s="4"/>
+      <c r="BK20" s="4"/>
+      <c r="BL20" s="4"/>
+      <c r="BM20" s="4"/>
+      <c r="BN20" s="4"/>
+      <c r="BO20" s="4"/>
+      <c r="BP20" s="4"/>
+      <c r="BQ20" s="4"/>
+      <c r="BR20" s="4"/>
+      <c r="BS20" s="4"/>
+      <c r="BT20" s="4"/>
+      <c r="BU20" s="4"/>
+      <c r="BV20" s="4"/>
+      <c r="BW20" s="4"/>
+      <c r="BX20" s="4"/>
+      <c r="BY20" s="4"/>
+      <c r="BZ20" s="4"/>
+      <c r="CA20" s="4"/>
+      <c r="CB20" s="4"/>
+      <c r="CC20" s="4"/>
+      <c r="CD20" s="4"/>
+      <c r="CE20" s="4"/>
+      <c r="CF20" s="4"/>
+      <c r="CG20" s="4"/>
+      <c r="CH20" s="4"/>
+      <c r="CI20" s="4"/>
+      <c r="CJ20" s="4"/>
+      <c r="CK20" s="4"/>
+      <c r="CL20" s="4"/>
+      <c r="CM20" s="4"/>
+      <c r="CN20" s="4"/>
+      <c r="CO20" s="4"/>
+      <c r="CP20" s="4"/>
+      <c r="CQ20" s="4"/>
+      <c r="CR20" s="4"/>
+      <c r="CS20" s="4"/>
+      <c r="CT20" s="4"/>
+      <c r="CU20" s="4"/>
+      <c r="CV20" s="4"/>
+      <c r="CW20" s="4"/>
+      <c r="CX20" s="4"/>
+      <c r="CY20" s="4"/>
+      <c r="CZ20" s="4"/>
+      <c r="DA20" s="4"/>
+      <c r="DB20" s="4"/>
+      <c r="DC20" s="4"/>
+      <c r="DD20" s="4"/>
+      <c r="DE20" s="4"/>
+      <c r="DF20" s="4"/>
+      <c r="DG20" s="4"/>
+      <c r="DH20" s="4"/>
+      <c r="DI20" s="4"/>
+      <c r="DJ20" s="4"/>
+      <c r="DK20" s="4"/>
+      <c r="DL20" s="4"/>
+      <c r="DM20" s="4"/>
+      <c r="DN20" s="4"/>
+      <c r="DO20" s="4"/>
+      <c r="DP20" s="4"/>
+      <c r="DQ20" s="4"/>
+      <c r="DR20" s="4"/>
+      <c r="DS20" s="4"/>
+      <c r="DT20" s="4"/>
+      <c r="DU20" s="4"/>
+      <c r="DV20" s="4"/>
+      <c r="DW20" s="4"/>
+      <c r="DX20" s="4"/>
+      <c r="DY20" s="4"/>
+      <c r="DZ20" s="4"/>
+      <c r="EA20" s="4"/>
+      <c r="EB20" s="4"/>
+      <c r="EC20" s="4"/>
+      <c r="ED20" s="4"/>
+      <c r="EE20" s="4"/>
+      <c r="EF20" s="4"/>
+      <c r="EG20" s="4"/>
+      <c r="EH20" s="4"/>
+      <c r="EI20" s="4"/>
+      <c r="EJ20" s="4"/>
+      <c r="EK20" s="4"/>
+      <c r="EL20" s="4"/>
+      <c r="EM20" s="4"/>
+      <c r="EN20" s="4"/>
+      <c r="EO20" s="4"/>
+      <c r="EP20" s="4"/>
+      <c r="EQ20" s="4"/>
+      <c r="ER20" s="4"/>
+      <c r="ES20" s="4"/>
+      <c r="ET20" s="4"/>
+      <c r="EU20" s="4"/>
+      <c r="EV20" s="4"/>
+      <c r="EW20" s="4"/>
+      <c r="EX20" s="4"/>
+      <c r="EY20" s="4"/>
+      <c r="EZ20" s="4"/>
+      <c r="FA20" s="4"/>
+      <c r="FB20" s="4"/>
+      <c r="FC20" s="4"/>
+      <c r="FD20" s="4"/>
+      <c r="FE20" s="4"/>
+      <c r="FF20" s="4"/>
+      <c r="FG20" s="4"/>
+      <c r="FH20" s="4"/>
+      <c r="FI20" s="4"/>
+      <c r="FJ20" s="4"/>
+      <c r="FK20" s="4"/>
+      <c r="FL20" s="4"/>
+      <c r="FM20" s="4"/>
+      <c r="FN20" s="4"/>
+      <c r="FO20" s="4"/>
+      <c r="FP20" s="4"/>
+      <c r="FQ20" s="4"/>
+      <c r="FR20" s="4"/>
+      <c r="FS20" s="4"/>
+      <c r="FT20" s="4"/>
+      <c r="FU20" s="4"/>
+      <c r="FV20" s="4"/>
+      <c r="FW20" s="4"/>
+      <c r="FX20" s="4"/>
+      <c r="FY20" s="4"/>
+      <c r="FZ20" s="4"/>
     </row>
     <row r="21" spans="1:182" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D21">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="E21">
         <v>11</v>
       </c>
       <c r="F21">
+        <v>3</v>
+      </c>
+      <c r="G21">
+        <v>21.77</v>
+      </c>
+      <c r="H21">
+        <v>49.19</v>
+      </c>
+      <c r="I21">
+        <v>62.09</v>
+      </c>
+      <c r="J21">
+        <v>3.67</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+      <c r="Y21" s="4"/>
+      <c r="Z21" s="4"/>
+      <c r="AA21" s="4"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+      <c r="AG21" s="4"/>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="4"/>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AL21" s="4"/>
+      <c r="AM21" s="4"/>
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="4"/>
+      <c r="AQ21" s="4"/>
+      <c r="AR21" s="4"/>
+      <c r="AS21" s="4"/>
+      <c r="AT21" s="4"/>
+      <c r="AU21" s="4"/>
+      <c r="AV21" s="4"/>
+      <c r="AW21" s="4"/>
+      <c r="AX21" s="4"/>
+      <c r="AY21" s="4"/>
+      <c r="AZ21" s="4"/>
+      <c r="BA21" s="4"/>
+      <c r="BB21" s="4"/>
+      <c r="BC21" s="4"/>
+      <c r="BD21" s="4"/>
+      <c r="BE21" s="4"/>
+      <c r="BF21" s="4"/>
+      <c r="BG21" s="4"/>
+      <c r="BH21" s="4"/>
+      <c r="BI21" s="4"/>
+      <c r="BJ21" s="4"/>
+      <c r="BK21" s="4"/>
+      <c r="BL21" s="4"/>
+      <c r="BM21" s="4"/>
+      <c r="BN21" s="4"/>
+      <c r="BO21" s="4"/>
+      <c r="BP21" s="4"/>
+      <c r="BQ21" s="4"/>
+      <c r="BR21" s="4"/>
+      <c r="BS21" s="4"/>
+      <c r="BT21" s="4"/>
+      <c r="BU21" s="4"/>
+      <c r="BV21" s="4"/>
+      <c r="BW21" s="4"/>
+      <c r="BX21" s="4"/>
+      <c r="BY21" s="4"/>
+      <c r="BZ21" s="4"/>
+      <c r="CA21" s="4"/>
+      <c r="CB21" s="4"/>
+      <c r="CC21" s="4"/>
+      <c r="CD21" s="4"/>
+      <c r="CE21" s="4"/>
+      <c r="CF21" s="4"/>
+      <c r="CG21" s="4"/>
+      <c r="CH21" s="4"/>
+      <c r="CI21" s="4"/>
+      <c r="CJ21" s="4"/>
+      <c r="CK21" s="4"/>
+      <c r="CL21" s="4"/>
+      <c r="CM21" s="4"/>
+      <c r="CN21" s="4"/>
+      <c r="CO21" s="4"/>
+      <c r="CP21" s="4"/>
+      <c r="CQ21" s="4"/>
+      <c r="CR21" s="4"/>
+      <c r="CS21" s="4"/>
+      <c r="CT21" s="4"/>
+      <c r="CU21" s="4"/>
+      <c r="CV21" s="4"/>
+      <c r="CW21" s="4"/>
+      <c r="CX21" s="4"/>
+      <c r="CY21" s="4"/>
+      <c r="CZ21" s="4"/>
+      <c r="DA21" s="4"/>
+      <c r="DB21" s="4"/>
+      <c r="DC21" s="4"/>
+      <c r="DD21" s="4"/>
+      <c r="DE21" s="4"/>
+      <c r="DF21" s="4"/>
+      <c r="DG21" s="4"/>
+      <c r="DH21" s="4"/>
+      <c r="DI21" s="4"/>
+      <c r="DJ21" s="4"/>
+      <c r="DK21" s="4"/>
+      <c r="DL21" s="4"/>
+      <c r="DM21" s="4"/>
+      <c r="DN21" s="4"/>
+      <c r="DO21" s="4"/>
+      <c r="DP21" s="4"/>
+      <c r="DQ21" s="4"/>
+      <c r="DR21" s="4"/>
+      <c r="DS21" s="4"/>
+      <c r="DT21" s="4"/>
+      <c r="DU21" s="4"/>
+      <c r="DV21" s="4"/>
+      <c r="DW21" s="4"/>
+      <c r="DX21" s="4"/>
+      <c r="DY21" s="4"/>
+      <c r="DZ21" s="4"/>
+      <c r="EA21" s="4"/>
+      <c r="EB21" s="4"/>
+      <c r="EC21" s="4"/>
+      <c r="ED21" s="4"/>
+      <c r="EE21" s="4"/>
+      <c r="EF21" s="4"/>
+      <c r="EG21" s="4"/>
+      <c r="EH21" s="4"/>
+      <c r="EI21" s="4"/>
+      <c r="EJ21" s="4"/>
+      <c r="EK21" s="4"/>
+      <c r="EL21" s="4"/>
+      <c r="EM21" s="4"/>
+      <c r="EN21" s="4"/>
+      <c r="EO21" s="4"/>
+      <c r="EP21" s="4"/>
+      <c r="EQ21" s="4"/>
+      <c r="ER21" s="4"/>
+      <c r="ES21" s="4"/>
+      <c r="ET21" s="4"/>
+      <c r="EU21" s="4"/>
+      <c r="EV21" s="4"/>
+      <c r="EW21" s="4"/>
+      <c r="EX21" s="4"/>
+      <c r="EY21" s="4"/>
+      <c r="EZ21" s="4"/>
+      <c r="FA21" s="4"/>
+      <c r="FB21" s="4"/>
+      <c r="FC21" s="4"/>
+      <c r="FD21" s="4"/>
+      <c r="FE21" s="4"/>
+      <c r="FF21" s="4"/>
+      <c r="FG21" s="4"/>
+      <c r="FH21" s="4"/>
+      <c r="FI21" s="4"/>
+      <c r="FJ21" s="4"/>
+      <c r="FK21" s="4"/>
+      <c r="FL21" s="4"/>
+      <c r="FM21" s="4"/>
+      <c r="FN21" s="4"/>
+      <c r="FO21" s="4"/>
+      <c r="FP21" s="4"/>
+      <c r="FQ21" s="4"/>
+      <c r="FR21" s="4"/>
+      <c r="FS21" s="4"/>
+      <c r="FT21" s="4"/>
+      <c r="FU21" s="4"/>
+      <c r="FV21" s="4"/>
+      <c r="FW21" s="4"/>
+      <c r="FX21" s="4"/>
+      <c r="FY21" s="4"/>
+      <c r="FZ21" s="4"/>
+    </row>
+    <row r="22" spans="1:182" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>2</v>
       </c>
-      <c r="G21">
+      <c r="B22">
+        <v>2019</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>25</v>
+      </c>
+      <c r="E22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>2.98</v>
+      </c>
+      <c r="H22">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="I22">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="J22">
+        <v>3.33</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="2"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="2"/>
+      <c r="AI22" s="2"/>
+      <c r="AJ22" s="2"/>
+      <c r="AK22" s="2"/>
+      <c r="AL22" s="2"/>
+      <c r="AM22" s="2"/>
+      <c r="AN22" s="2"/>
+      <c r="AO22" s="2"/>
+      <c r="AP22" s="2"/>
+      <c r="AQ22" s="2"/>
+      <c r="AR22" s="2"/>
+      <c r="AS22" s="2"/>
+      <c r="AT22" s="2"/>
+      <c r="AU22" s="2"/>
+      <c r="AV22" s="2"/>
+      <c r="AW22" s="2"/>
+      <c r="AX22" s="2"/>
+      <c r="AY22" s="2"/>
+      <c r="AZ22" s="2"/>
+      <c r="BA22" s="2"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="2"/>
+      <c r="BD22" s="2"/>
+      <c r="BE22" s="2"/>
+      <c r="BF22" s="2"/>
+      <c r="BG22" s="2"/>
+      <c r="BH22" s="2"/>
+      <c r="BI22" s="2"/>
+      <c r="BJ22" s="2"/>
+      <c r="BK22" s="2"/>
+      <c r="BL22" s="2"/>
+      <c r="BM22" s="2"/>
+      <c r="BN22" s="2"/>
+      <c r="BO22" s="2"/>
+      <c r="BP22" s="2"/>
+      <c r="BQ22" s="2"/>
+      <c r="BR22" s="2"/>
+      <c r="BS22" s="2"/>
+      <c r="BT22" s="2"/>
+      <c r="BU22" s="2"/>
+      <c r="BV22" s="2"/>
+      <c r="BW22" s="2"/>
+      <c r="BX22" s="2"/>
+      <c r="BY22" s="2"/>
+      <c r="BZ22" s="2"/>
+      <c r="CA22" s="2"/>
+      <c r="CB22" s="2"/>
+      <c r="CC22" s="2"/>
+      <c r="CD22" s="2"/>
+      <c r="CE22" s="2"/>
+      <c r="CF22" s="2"/>
+      <c r="CG22" s="2"/>
+      <c r="CH22" s="2"/>
+      <c r="CI22" s="2"/>
+      <c r="CJ22" s="2"/>
+      <c r="CK22" s="2"/>
+      <c r="CL22" s="2"/>
+      <c r="CM22" s="2"/>
+      <c r="CN22" s="2"/>
+      <c r="CO22" s="2"/>
+      <c r="CP22" s="2"/>
+      <c r="CQ22" s="2"/>
+      <c r="CR22" s="2"/>
+      <c r="CS22" s="2"/>
+      <c r="CT22" s="2"/>
+      <c r="CU22" s="2"/>
+      <c r="CV22" s="2"/>
+      <c r="CW22" s="2"/>
+      <c r="CX22" s="2"/>
+      <c r="CY22" s="2"/>
+      <c r="CZ22" s="2"/>
+      <c r="DA22" s="2"/>
+      <c r="DB22" s="2"/>
+      <c r="DC22" s="2"/>
+      <c r="DD22" s="2"/>
+      <c r="DE22" s="2"/>
+      <c r="DF22" s="2"/>
+      <c r="DG22" s="2"/>
+      <c r="DH22" s="2"/>
+      <c r="DI22" s="2"/>
+      <c r="DJ22" s="2"/>
+      <c r="DK22" s="2"/>
+      <c r="DL22" s="2"/>
+      <c r="DM22" s="2"/>
+      <c r="DN22" s="2"/>
+      <c r="DO22" s="2"/>
+      <c r="DP22" s="2"/>
+      <c r="DQ22" s="2"/>
+      <c r="DR22" s="2"/>
+      <c r="DS22" s="2"/>
+      <c r="DT22" s="2"/>
+      <c r="DU22" s="2"/>
+      <c r="DV22" s="2"/>
+      <c r="DW22" s="2"/>
+      <c r="DX22" s="2"/>
+      <c r="DY22" s="2"/>
+      <c r="DZ22" s="2"/>
+      <c r="EA22" s="2"/>
+      <c r="EB22" s="2"/>
+      <c r="EC22" s="2"/>
+      <c r="ED22" s="2"/>
+      <c r="EE22" s="2"/>
+      <c r="EF22" s="2"/>
+      <c r="EG22" s="2"/>
+      <c r="EH22" s="2"/>
+      <c r="EI22" s="2"/>
+      <c r="EJ22" s="2"/>
+      <c r="EK22" s="2"/>
+      <c r="EL22" s="2"/>
+      <c r="EM22" s="2"/>
+      <c r="EN22" s="2"/>
+      <c r="EO22" s="2"/>
+      <c r="EP22" s="2"/>
+      <c r="EQ22" s="2"/>
+      <c r="ER22" s="2"/>
+      <c r="ES22" s="2"/>
+      <c r="ET22" s="2"/>
+      <c r="EU22" s="2"/>
+      <c r="EV22" s="2"/>
+      <c r="EW22" s="2"/>
+      <c r="EX22" s="2"/>
+      <c r="EY22" s="2"/>
+      <c r="EZ22" s="2"/>
+      <c r="FA22" s="2"/>
+      <c r="FB22" s="2"/>
+      <c r="FC22" s="2"/>
+      <c r="FD22" s="2"/>
+      <c r="FE22" s="2"/>
+      <c r="FF22" s="2"/>
+      <c r="FG22" s="2"/>
+      <c r="FH22" s="2"/>
+      <c r="FI22" s="2"/>
+      <c r="FJ22" s="2"/>
+      <c r="FK22" s="2"/>
+      <c r="FL22" s="2"/>
+      <c r="FM22" s="2"/>
+      <c r="FN22" s="2"/>
+      <c r="FO22" s="2"/>
+      <c r="FP22" s="2"/>
+      <c r="FQ22" s="2"/>
+      <c r="FR22" s="2"/>
+      <c r="FS22" s="2"/>
+      <c r="FT22" s="2"/>
+      <c r="FU22" s="2"/>
+      <c r="FV22" s="2"/>
+      <c r="FW22" s="2"/>
+      <c r="FX22" s="2"/>
+      <c r="FY22" s="2"/>
+      <c r="FZ22" s="2"/>
+    </row>
+    <row r="23" spans="1:182" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>2019</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>75.319999999999993</v>
+      </c>
+      <c r="I23">
+        <v>60.13</v>
+      </c>
+      <c r="J23">
+        <v>1.67</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="2"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="2"/>
+      <c r="AI23" s="2"/>
+      <c r="AJ23" s="2"/>
+      <c r="AK23" s="2"/>
+      <c r="AL23" s="2"/>
+      <c r="AM23" s="2"/>
+      <c r="AN23" s="2"/>
+      <c r="AO23" s="2"/>
+      <c r="AP23" s="2"/>
+      <c r="AQ23" s="2"/>
+      <c r="AR23" s="2"/>
+      <c r="AS23" s="2"/>
+      <c r="AT23" s="2"/>
+      <c r="AU23" s="2"/>
+      <c r="AV23" s="2"/>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="2"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="2"/>
+      <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="2"/>
+      <c r="BD23" s="2"/>
+      <c r="BE23" s="2"/>
+      <c r="BF23" s="2"/>
+      <c r="BG23" s="2"/>
+      <c r="BH23" s="2"/>
+      <c r="BI23" s="2"/>
+      <c r="BJ23" s="2"/>
+      <c r="BK23" s="2"/>
+      <c r="BL23" s="2"/>
+      <c r="BM23" s="2"/>
+      <c r="BN23" s="2"/>
+      <c r="BO23" s="2"/>
+      <c r="BP23" s="2"/>
+      <c r="BQ23" s="2"/>
+      <c r="BR23" s="2"/>
+      <c r="BS23" s="2"/>
+      <c r="BT23" s="2"/>
+      <c r="BU23" s="2"/>
+      <c r="BV23" s="2"/>
+      <c r="BW23" s="2"/>
+      <c r="BX23" s="2"/>
+      <c r="BY23" s="2"/>
+      <c r="BZ23" s="2"/>
+      <c r="CA23" s="2"/>
+      <c r="CB23" s="2"/>
+      <c r="CC23" s="2"/>
+      <c r="CD23" s="2"/>
+      <c r="CE23" s="2"/>
+      <c r="CF23" s="2"/>
+      <c r="CG23" s="2"/>
+      <c r="CH23" s="2"/>
+      <c r="CI23" s="2"/>
+      <c r="CJ23" s="2"/>
+      <c r="CK23" s="2"/>
+      <c r="CL23" s="2"/>
+      <c r="CM23" s="2"/>
+      <c r="CN23" s="2"/>
+      <c r="CO23" s="2"/>
+      <c r="CP23" s="2"/>
+      <c r="CQ23" s="2"/>
+      <c r="CR23" s="2"/>
+      <c r="CS23" s="2"/>
+      <c r="CT23" s="2"/>
+      <c r="CU23" s="2"/>
+      <c r="CV23" s="2"/>
+      <c r="CW23" s="2"/>
+      <c r="CX23" s="2"/>
+      <c r="CY23" s="2"/>
+      <c r="CZ23" s="2"/>
+      <c r="DA23" s="2"/>
+      <c r="DB23" s="2"/>
+      <c r="DC23" s="2"/>
+      <c r="DD23" s="2"/>
+      <c r="DE23" s="2"/>
+      <c r="DF23" s="2"/>
+      <c r="DG23" s="2"/>
+      <c r="DH23" s="2"/>
+      <c r="DI23" s="2"/>
+      <c r="DJ23" s="2"/>
+      <c r="DK23" s="2"/>
+      <c r="DL23" s="2"/>
+      <c r="DM23" s="2"/>
+      <c r="DN23" s="2"/>
+      <c r="DO23" s="2"/>
+      <c r="DP23" s="2"/>
+      <c r="DQ23" s="2"/>
+      <c r="DR23" s="2"/>
+      <c r="DS23" s="2"/>
+      <c r="DT23" s="2"/>
+      <c r="DU23" s="2"/>
+      <c r="DV23" s="2"/>
+      <c r="DW23" s="2"/>
+      <c r="DX23" s="2"/>
+      <c r="DY23" s="2"/>
+      <c r="DZ23" s="2"/>
+      <c r="EA23" s="2"/>
+      <c r="EB23" s="2"/>
+      <c r="EC23" s="2"/>
+      <c r="ED23" s="2"/>
+      <c r="EE23" s="2"/>
+      <c r="EF23" s="2"/>
+      <c r="EG23" s="2"/>
+      <c r="EH23" s="2"/>
+      <c r="EI23" s="2"/>
+      <c r="EJ23" s="2"/>
+      <c r="EK23" s="2"/>
+      <c r="EL23" s="2"/>
+      <c r="EM23" s="2"/>
+      <c r="EN23" s="2"/>
+      <c r="EO23" s="2"/>
+      <c r="EP23" s="2"/>
+      <c r="EQ23" s="2"/>
+      <c r="ER23" s="2"/>
+      <c r="ES23" s="2"/>
+      <c r="ET23" s="2"/>
+      <c r="EU23" s="2"/>
+      <c r="EV23" s="2"/>
+      <c r="EW23" s="2"/>
+      <c r="EX23" s="2"/>
+      <c r="EY23" s="2"/>
+      <c r="EZ23" s="2"/>
+      <c r="FA23" s="2"/>
+      <c r="FB23" s="2"/>
+      <c r="FC23" s="2"/>
+      <c r="FD23" s="2"/>
+      <c r="FE23" s="2"/>
+      <c r="FF23" s="2"/>
+      <c r="FG23" s="2"/>
+      <c r="FH23" s="2"/>
+      <c r="FI23" s="2"/>
+      <c r="FJ23" s="2"/>
+      <c r="FK23" s="2"/>
+      <c r="FL23" s="2"/>
+      <c r="FM23" s="2"/>
+      <c r="FN23" s="2"/>
+      <c r="FO23" s="2"/>
+      <c r="FP23" s="2"/>
+      <c r="FQ23" s="2"/>
+      <c r="FR23" s="2"/>
+      <c r="FS23" s="2"/>
+      <c r="FT23" s="2"/>
+      <c r="FU23" s="2"/>
+      <c r="FV23" s="2"/>
+      <c r="FW23" s="2"/>
+      <c r="FX23" s="2"/>
+      <c r="FY23" s="2"/>
+      <c r="FZ23" s="2"/>
+    </row>
+    <row r="24" spans="1:182" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2019</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>1.47</v>
+      </c>
+      <c r="H24">
+        <v>32.35</v>
+      </c>
+      <c r="I24">
+        <v>79.41</v>
+      </c>
+      <c r="J24">
+        <v>2.33</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="2"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="2"/>
+      <c r="AI24" s="2"/>
+      <c r="AJ24" s="2"/>
+      <c r="AK24" s="2"/>
+      <c r="AL24" s="2"/>
+      <c r="AM24" s="2"/>
+      <c r="AN24" s="2"/>
+      <c r="AO24" s="2"/>
+      <c r="AP24" s="2"/>
+      <c r="AQ24" s="2"/>
+      <c r="AR24" s="2"/>
+      <c r="AS24" s="2"/>
+      <c r="AT24" s="2"/>
+      <c r="AU24" s="2"/>
+      <c r="AV24" s="2"/>
+      <c r="AW24" s="2"/>
+      <c r="AX24" s="2"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="2"/>
+      <c r="BA24" s="2"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="2"/>
+      <c r="BD24" s="2"/>
+      <c r="BE24" s="2"/>
+      <c r="BF24" s="2"/>
+      <c r="BG24" s="2"/>
+      <c r="BH24" s="2"/>
+      <c r="BI24" s="2"/>
+      <c r="BJ24" s="2"/>
+      <c r="BK24" s="2"/>
+      <c r="BL24" s="2"/>
+      <c r="BM24" s="2"/>
+      <c r="BN24" s="2"/>
+      <c r="BO24" s="2"/>
+      <c r="BP24" s="2"/>
+      <c r="BQ24" s="2"/>
+      <c r="BR24" s="2"/>
+      <c r="BS24" s="2"/>
+      <c r="BT24" s="2"/>
+      <c r="BU24" s="2"/>
+      <c r="BV24" s="2"/>
+      <c r="BW24" s="2"/>
+      <c r="BX24" s="2"/>
+      <c r="BY24" s="2"/>
+      <c r="BZ24" s="2"/>
+      <c r="CA24" s="2"/>
+      <c r="CB24" s="2"/>
+      <c r="CC24" s="2"/>
+      <c r="CD24" s="2"/>
+      <c r="CE24" s="2"/>
+      <c r="CF24" s="2"/>
+      <c r="CG24" s="2"/>
+      <c r="CH24" s="2"/>
+      <c r="CI24" s="2"/>
+      <c r="CJ24" s="2"/>
+      <c r="CK24" s="2"/>
+      <c r="CL24" s="2"/>
+      <c r="CM24" s="2"/>
+      <c r="CN24" s="2"/>
+      <c r="CO24" s="2"/>
+      <c r="CP24" s="2"/>
+      <c r="CQ24" s="2"/>
+      <c r="CR24" s="2"/>
+      <c r="CS24" s="2"/>
+      <c r="CT24" s="2"/>
+      <c r="CU24" s="2"/>
+      <c r="CV24" s="2"/>
+      <c r="CW24" s="2"/>
+      <c r="CX24" s="2"/>
+      <c r="CY24" s="2"/>
+      <c r="CZ24" s="2"/>
+      <c r="DA24" s="2"/>
+      <c r="DB24" s="2"/>
+      <c r="DC24" s="2"/>
+      <c r="DD24" s="2"/>
+      <c r="DE24" s="2"/>
+      <c r="DF24" s="2"/>
+      <c r="DG24" s="2"/>
+      <c r="DH24" s="2"/>
+      <c r="DI24" s="2"/>
+      <c r="DJ24" s="2"/>
+      <c r="DK24" s="2"/>
+      <c r="DL24" s="2"/>
+      <c r="DM24" s="2"/>
+      <c r="DN24" s="2"/>
+      <c r="DO24" s="2"/>
+      <c r="DP24" s="2"/>
+      <c r="DQ24" s="2"/>
+      <c r="DR24" s="2"/>
+      <c r="DS24" s="2"/>
+      <c r="DT24" s="2"/>
+      <c r="DU24" s="2"/>
+      <c r="DV24" s="2"/>
+      <c r="DW24" s="2"/>
+      <c r="DX24" s="2"/>
+      <c r="DY24" s="2"/>
+      <c r="DZ24" s="2"/>
+      <c r="EA24" s="2"/>
+      <c r="EB24" s="2"/>
+      <c r="EC24" s="2"/>
+      <c r="ED24" s="2"/>
+      <c r="EE24" s="2"/>
+      <c r="EF24" s="2"/>
+      <c r="EG24" s="2"/>
+      <c r="EH24" s="2"/>
+      <c r="EI24" s="2"/>
+      <c r="EJ24" s="2"/>
+      <c r="EK24" s="2"/>
+      <c r="EL24" s="2"/>
+      <c r="EM24" s="2"/>
+      <c r="EN24" s="2"/>
+      <c r="EO24" s="2"/>
+      <c r="EP24" s="2"/>
+      <c r="EQ24" s="2"/>
+      <c r="ER24" s="2"/>
+      <c r="ES24" s="2"/>
+      <c r="ET24" s="2"/>
+      <c r="EU24" s="2"/>
+      <c r="EV24" s="2"/>
+      <c r="EW24" s="2"/>
+      <c r="EX24" s="2"/>
+      <c r="EY24" s="2"/>
+      <c r="EZ24" s="2"/>
+      <c r="FA24" s="2"/>
+      <c r="FB24" s="2"/>
+      <c r="FC24" s="2"/>
+      <c r="FD24" s="2"/>
+      <c r="FE24" s="2"/>
+      <c r="FF24" s="2"/>
+      <c r="FG24" s="2"/>
+      <c r="FH24" s="2"/>
+      <c r="FI24" s="2"/>
+      <c r="FJ24" s="2"/>
+      <c r="FK24" s="2"/>
+      <c r="FL24" s="2"/>
+      <c r="FM24" s="2"/>
+      <c r="FN24" s="2"/>
+      <c r="FO24" s="2"/>
+      <c r="FP24" s="2"/>
+      <c r="FQ24" s="2"/>
+      <c r="FR24" s="2"/>
+      <c r="FS24" s="2"/>
+      <c r="FT24" s="2"/>
+      <c r="FU24" s="2"/>
+      <c r="FV24" s="2"/>
+      <c r="FW24" s="2"/>
+      <c r="FX24" s="2"/>
+      <c r="FY24" s="2"/>
+      <c r="FZ24" s="2"/>
+    </row>
+    <row r="25" spans="1:182" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>2019</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>25</v>
+      </c>
+      <c r="E25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
         <v>37.299999999999997</v>
       </c>
-      <c r="H21">
+      <c r="H25">
         <v>20.63</v>
       </c>
-      <c r="I21">
+      <c r="I25">
         <v>89.68</v>
       </c>
-      <c r="J21">
+      <c r="J25">
         <v>4.33</v>
       </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-      <c r="W21" s="2"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="2"/>
-      <c r="Z21" s="2"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="2"/>
-      <c r="AD21" s="2"/>
-      <c r="AE21" s="2"/>
-      <c r="AF21" s="2"/>
-      <c r="AG21" s="2"/>
-      <c r="AH21" s="2"/>
-      <c r="AI21" s="2"/>
-      <c r="AJ21" s="2"/>
-      <c r="AK21" s="2"/>
-      <c r="AL21" s="2"/>
-      <c r="AM21" s="2"/>
-      <c r="AN21" s="2"/>
-      <c r="AO21" s="2"/>
-      <c r="AP21" s="2"/>
-      <c r="AQ21" s="2"/>
-      <c r="AR21" s="2"/>
-      <c r="AS21" s="2"/>
-      <c r="AT21" s="2"/>
-      <c r="AU21" s="2"/>
-      <c r="AV21" s="2"/>
-      <c r="AW21" s="2"/>
-      <c r="AX21" s="2"/>
-      <c r="AY21" s="2"/>
-      <c r="AZ21" s="2"/>
-      <c r="BA21" s="2"/>
-      <c r="BB21" s="2"/>
-      <c r="BC21" s="2"/>
-      <c r="BD21" s="2"/>
-      <c r="BE21" s="2"/>
-      <c r="BF21" s="2"/>
-      <c r="BG21" s="2"/>
-      <c r="BH21" s="2"/>
-      <c r="BI21" s="2"/>
-      <c r="BJ21" s="2"/>
-      <c r="BK21" s="2"/>
-      <c r="BL21" s="2"/>
-      <c r="BM21" s="2"/>
-      <c r="BN21" s="2"/>
-      <c r="BO21" s="2"/>
-      <c r="BP21" s="2"/>
-      <c r="BQ21" s="2"/>
-      <c r="BR21" s="2"/>
-      <c r="BS21" s="2"/>
-      <c r="BT21" s="2"/>
-      <c r="BU21" s="2"/>
-      <c r="BV21" s="2"/>
-      <c r="BW21" s="2"/>
-      <c r="BX21" s="2"/>
-      <c r="BY21" s="2"/>
-      <c r="BZ21" s="2"/>
-      <c r="CA21" s="2"/>
-      <c r="CB21" s="2"/>
-      <c r="CC21" s="2"/>
-      <c r="CD21" s="2"/>
-      <c r="CE21" s="2"/>
-      <c r="CF21" s="2"/>
-      <c r="CG21" s="2"/>
-      <c r="CH21" s="2"/>
-      <c r="CI21" s="2"/>
-      <c r="CJ21" s="2"/>
-      <c r="CK21" s="2"/>
-      <c r="CL21" s="2"/>
-      <c r="CM21" s="2"/>
-      <c r="CN21" s="2"/>
-      <c r="CO21" s="2"/>
-      <c r="CP21" s="2"/>
-      <c r="CQ21" s="2"/>
-      <c r="CR21" s="2"/>
-      <c r="CS21" s="2"/>
-      <c r="CT21" s="2"/>
-      <c r="CU21" s="2"/>
-      <c r="CV21" s="2"/>
-      <c r="CW21" s="2"/>
-      <c r="CX21" s="2"/>
-      <c r="CY21" s="2"/>
-      <c r="CZ21" s="2"/>
-      <c r="DA21" s="2"/>
-      <c r="DB21" s="2"/>
-      <c r="DC21" s="2"/>
-      <c r="DD21" s="2"/>
-      <c r="DE21" s="2"/>
-      <c r="DF21" s="2"/>
-      <c r="DG21" s="2"/>
-      <c r="DH21" s="2"/>
-      <c r="DI21" s="2"/>
-      <c r="DJ21" s="2"/>
-      <c r="DK21" s="2"/>
-      <c r="DL21" s="2"/>
-      <c r="DM21" s="2"/>
-      <c r="DN21" s="2"/>
-      <c r="DO21" s="2"/>
-      <c r="DP21" s="2"/>
-      <c r="DQ21" s="2"/>
-      <c r="DR21" s="2"/>
-      <c r="DS21" s="2"/>
-      <c r="DT21" s="2"/>
-      <c r="DU21" s="2"/>
-      <c r="DV21" s="2"/>
-      <c r="DW21" s="2"/>
-      <c r="DX21" s="2"/>
-      <c r="DY21" s="2"/>
-      <c r="DZ21" s="2"/>
-      <c r="EA21" s="2"/>
-      <c r="EB21" s="2"/>
-      <c r="EC21" s="2"/>
-      <c r="ED21" s="2"/>
-      <c r="EE21" s="2"/>
-      <c r="EF21" s="2"/>
-      <c r="EG21" s="2"/>
-      <c r="EH21" s="2"/>
-      <c r="EI21" s="2"/>
-      <c r="EJ21" s="2"/>
-      <c r="EK21" s="2"/>
-      <c r="EL21" s="2"/>
-      <c r="EM21" s="2"/>
-      <c r="EN21" s="2"/>
-      <c r="EO21" s="2"/>
-      <c r="EP21" s="2"/>
-      <c r="EQ21" s="2"/>
-      <c r="ER21" s="2"/>
-      <c r="ES21" s="2"/>
-      <c r="ET21" s="2"/>
-      <c r="EU21" s="2"/>
-      <c r="EV21" s="2"/>
-      <c r="EW21" s="2"/>
-      <c r="EX21" s="2"/>
-      <c r="EY21" s="2"/>
-      <c r="EZ21" s="2"/>
-      <c r="FA21" s="2"/>
-      <c r="FB21" s="2"/>
-      <c r="FC21" s="2"/>
-      <c r="FD21" s="2"/>
-      <c r="FE21" s="2"/>
-      <c r="FF21" s="2"/>
-      <c r="FG21" s="2"/>
-      <c r="FH21" s="2"/>
-      <c r="FI21" s="2"/>
-      <c r="FJ21" s="2"/>
-      <c r="FK21" s="2"/>
-      <c r="FL21" s="2"/>
-      <c r="FM21" s="2"/>
-      <c r="FN21" s="2"/>
-      <c r="FO21" s="2"/>
-      <c r="FP21" s="2"/>
-      <c r="FQ21" s="2"/>
-      <c r="FR21" s="2"/>
-      <c r="FS21" s="2"/>
-      <c r="FT21" s="2"/>
-      <c r="FU21" s="2"/>
-      <c r="FV21" s="2"/>
-      <c r="FW21" s="2"/>
-      <c r="FX21" s="2"/>
-      <c r="FY21" s="2"/>
-      <c r="FZ21" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="2"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="2"/>
+      <c r="AI25" s="2"/>
+      <c r="AJ25" s="2"/>
+      <c r="AK25" s="2"/>
+      <c r="AL25" s="2"/>
+      <c r="AM25" s="2"/>
+      <c r="AN25" s="2"/>
+      <c r="AO25" s="2"/>
+      <c r="AP25" s="2"/>
+      <c r="AQ25" s="2"/>
+      <c r="AR25" s="2"/>
+      <c r="AS25" s="2"/>
+      <c r="AT25" s="2"/>
+      <c r="AU25" s="2"/>
+      <c r="AV25" s="2"/>
+      <c r="AW25" s="2"/>
+      <c r="AX25" s="2"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="2"/>
+      <c r="BA25" s="2"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="2"/>
+      <c r="BD25" s="2"/>
+      <c r="BE25" s="2"/>
+      <c r="BF25" s="2"/>
+      <c r="BG25" s="2"/>
+      <c r="BH25" s="2"/>
+      <c r="BI25" s="2"/>
+      <c r="BJ25" s="2"/>
+      <c r="BK25" s="2"/>
+      <c r="BL25" s="2"/>
+      <c r="BM25" s="2"/>
+      <c r="BN25" s="2"/>
+      <c r="BO25" s="2"/>
+      <c r="BP25" s="2"/>
+      <c r="BQ25" s="2"/>
+      <c r="BR25" s="2"/>
+      <c r="BS25" s="2"/>
+      <c r="BT25" s="2"/>
+      <c r="BU25" s="2"/>
+      <c r="BV25" s="2"/>
+      <c r="BW25" s="2"/>
+      <c r="BX25" s="2"/>
+      <c r="BY25" s="2"/>
+      <c r="BZ25" s="2"/>
+      <c r="CA25" s="2"/>
+      <c r="CB25" s="2"/>
+      <c r="CC25" s="2"/>
+      <c r="CD25" s="2"/>
+      <c r="CE25" s="2"/>
+      <c r="CF25" s="2"/>
+      <c r="CG25" s="2"/>
+      <c r="CH25" s="2"/>
+      <c r="CI25" s="2"/>
+      <c r="CJ25" s="2"/>
+      <c r="CK25" s="2"/>
+      <c r="CL25" s="2"/>
+      <c r="CM25" s="2"/>
+      <c r="CN25" s="2"/>
+      <c r="CO25" s="2"/>
+      <c r="CP25" s="2"/>
+      <c r="CQ25" s="2"/>
+      <c r="CR25" s="2"/>
+      <c r="CS25" s="2"/>
+      <c r="CT25" s="2"/>
+      <c r="CU25" s="2"/>
+      <c r="CV25" s="2"/>
+      <c r="CW25" s="2"/>
+      <c r="CX25" s="2"/>
+      <c r="CY25" s="2"/>
+      <c r="CZ25" s="2"/>
+      <c r="DA25" s="2"/>
+      <c r="DB25" s="2"/>
+      <c r="DC25" s="2"/>
+      <c r="DD25" s="2"/>
+      <c r="DE25" s="2"/>
+      <c r="DF25" s="2"/>
+      <c r="DG25" s="2"/>
+      <c r="DH25" s="2"/>
+      <c r="DI25" s="2"/>
+      <c r="DJ25" s="2"/>
+      <c r="DK25" s="2"/>
+      <c r="DL25" s="2"/>
+      <c r="DM25" s="2"/>
+      <c r="DN25" s="2"/>
+      <c r="DO25" s="2"/>
+      <c r="DP25" s="2"/>
+      <c r="DQ25" s="2"/>
+      <c r="DR25" s="2"/>
+      <c r="DS25" s="2"/>
+      <c r="DT25" s="2"/>
+      <c r="DU25" s="2"/>
+      <c r="DV25" s="2"/>
+      <c r="DW25" s="2"/>
+      <c r="DX25" s="2"/>
+      <c r="DY25" s="2"/>
+      <c r="DZ25" s="2"/>
+      <c r="EA25" s="2"/>
+      <c r="EB25" s="2"/>
+      <c r="EC25" s="2"/>
+      <c r="ED25" s="2"/>
+      <c r="EE25" s="2"/>
+      <c r="EF25" s="2"/>
+      <c r="EG25" s="2"/>
+      <c r="EH25" s="2"/>
+      <c r="EI25" s="2"/>
+      <c r="EJ25" s="2"/>
+      <c r="EK25" s="2"/>
+      <c r="EL25" s="2"/>
+      <c r="EM25" s="2"/>
+      <c r="EN25" s="2"/>
+      <c r="EO25" s="2"/>
+      <c r="EP25" s="2"/>
+      <c r="EQ25" s="2"/>
+      <c r="ER25" s="2"/>
+      <c r="ES25" s="2"/>
+      <c r="ET25" s="2"/>
+      <c r="EU25" s="2"/>
+      <c r="EV25" s="2"/>
+      <c r="EW25" s="2"/>
+      <c r="EX25" s="2"/>
+      <c r="EY25" s="2"/>
+      <c r="EZ25" s="2"/>
+      <c r="FA25" s="2"/>
+      <c r="FB25" s="2"/>
+      <c r="FC25" s="2"/>
+      <c r="FD25" s="2"/>
+      <c r="FE25" s="2"/>
+      <c r="FF25" s="2"/>
+      <c r="FG25" s="2"/>
+      <c r="FH25" s="2"/>
+      <c r="FI25" s="2"/>
+      <c r="FJ25" s="2"/>
+      <c r="FK25" s="2"/>
+      <c r="FL25" s="2"/>
+      <c r="FM25" s="2"/>
+      <c r="FN25" s="2"/>
+      <c r="FO25" s="2"/>
+      <c r="FP25" s="2"/>
+      <c r="FQ25" s="2"/>
+      <c r="FR25" s="2"/>
+      <c r="FS25" s="2"/>
+      <c r="FT25" s="2"/>
+      <c r="FU25" s="2"/>
+      <c r="FV25" s="2"/>
+      <c r="FW25" s="2"/>
+      <c r="FX25" s="2"/>
+      <c r="FY25" s="2"/>
+      <c r="FZ25" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J1:FL1">

</xml_diff>